<commit_message>
added herbivory assay and fish survey datashe
</commit_message>
<xml_diff>
--- a/fishSurveys/data/Example BRUV Datasheet.xlsx
+++ b/fishSurveys/data/Example BRUV Datasheet.xlsx
@@ -1,28 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23145" windowHeight="9675"/>
+    <workbookView xWindow="-9630" yWindow="1950" windowWidth="23145" windowHeight="9675"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -70,30 +57,6 @@
     <t>Frame</t>
   </si>
   <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>TonySpecies_Cm</t>
-  </si>
-  <si>
-    <t>TonySpecies_Gn</t>
-  </si>
-  <si>
-    <t>TonySpecies_Sc</t>
-  </si>
-  <si>
-    <t>Rec_Count</t>
-  </si>
-  <si>
-    <t>Rec_Species_CM</t>
-  </si>
-  <si>
-    <t>Rec_Species_GN</t>
-  </si>
-  <si>
-    <t>Rec_Species_SC</t>
-  </si>
-  <si>
     <t>D_Time</t>
   </si>
   <si>
@@ -109,13 +72,37 @@
     <t>Transect</t>
   </si>
   <si>
-    <t>Reviewer1_Species_Cm</t>
-  </si>
-  <si>
-    <t>Reviewer1_Species_Gn</t>
-  </si>
-  <si>
-    <t>Reviewer1_Species_Sc</t>
+    <t>reviewer1SpeciesCm</t>
+  </si>
+  <si>
+    <t>reviewer1SpeciesGn</t>
+  </si>
+  <si>
+    <t>reviewer1SpeciesSc</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>reviewer2SpeciesCm</t>
+  </si>
+  <si>
+    <t>reviewer2SpeciesGn</t>
+  </si>
+  <si>
+    <t>reviewer2SpeciesSc</t>
+  </si>
+  <si>
+    <t>recCount</t>
+  </si>
+  <si>
+    <t>recSpeciesCm</t>
+  </si>
+  <si>
+    <t>recspeciesGn</t>
+  </si>
+  <si>
+    <t>recSpeciesSc</t>
   </si>
 </sst>
 </file>
@@ -214,9 +201,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -511,7 +495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -521,19 +505,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.140625" customWidth="1"/>
     <col min="13" max="13" width="16.42578125" customWidth="1"/>
     <col min="14" max="14" width="17.5703125" customWidth="1"/>
@@ -542,60 +526,60 @@
     <col min="17" max="17" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -605,6 +589,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>